<commit_message>
[FIX] sms bug when sending invoices
</commit_message>
<xml_diff>
--- a/oo_loyalty_savings/controllers/file.xlsx
+++ b/oo_loyalty_savings/controllers/file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Savings" sheetId="1" state="visible" r:id="rId2"/>
@@ -3665,8 +3665,8 @@
   </sheetPr>
   <dimension ref="A1:C627"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A543" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A561" activeCellId="0" sqref="A561"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A543" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A543" activeCellId="0" sqref="A543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10591,8 +10591,8 @@
   </sheetPr>
   <dimension ref="A1:C1104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>